<commit_message>
additions to the dictionary, it works now
</commit_message>
<xml_diff>
--- a/formative-elements/formative-elements.xlsx
+++ b/formative-elements/formative-elements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\usda.net\NRCS\Home\CASON\NRCS\Dylan.Beaudette\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\working_copies\SoilTaxonomy\formative-elements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A293382-B310-42E2-BEE4-C478900B2F37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C1A4ED-8493-46BF-97C3-E8EB6BB6C52D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9780" activeTab="2" xr2:uid="{728FE064-2144-4183-8F3E-A5F6ED41A2A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9780" activeTab="3" xr2:uid="{728FE064-2144-4183-8F3E-A5F6ED41A2A3}"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="454">
   <si>
     <t>element</t>
   </si>
@@ -1380,6 +1380,21 @@
   </si>
   <si>
     <t>xero</t>
+  </si>
+  <si>
+    <t>fluvaquentic</t>
+  </si>
+  <si>
+    <t>flood plain + water + entisol</t>
+  </si>
+  <si>
+    <t>wetter than typic subgroup, evidence of stratification</t>
+  </si>
+  <si>
+    <t>aridic</t>
+  </si>
+  <si>
+    <t>more aridic than typic subgroup</t>
   </si>
 </sst>
 </file>
@@ -1967,7 +1982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2406C0-4B40-475B-B0B2-D2A68ED4FB2E}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -2337,7 +2352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4648FD0D-CFBB-44A9-AB17-265531B6E9AE}">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -3308,10 +3323,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D2594B-1AEA-4072-B7F9-758DAECAB91F}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3563,41 +3578,41 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>452</v>
       </c>
       <c r="B14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>40</v>
+        <v>300</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>41</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="b">
         <v>0</v>
@@ -3606,32 +3621,32 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
         <v>0</v>
@@ -3640,32 +3655,32 @@
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B20" s="2" t="b">
         <v>0</v>
@@ -3674,32 +3689,32 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B22" s="2" t="b">
         <v>0</v>
@@ -3708,32 +3723,32 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>67</v>
+        <v>449</v>
       </c>
       <c r="B23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>68</v>
+        <v>450</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>69</v>
+        <v>451</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B24" s="2" t="b">
         <v>0</v>
@@ -3742,15 +3757,15 @@
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B25" s="2" t="b">
         <v>0</v>
@@ -3759,15 +3774,15 @@
         <v>0</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B26" s="2" t="b">
         <v>0</v>
@@ -3776,32 +3791,32 @@
         <v>0</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E27" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B28" s="2" t="b">
         <v>0</v>
@@ -3810,32 +3825,32 @@
         <v>0</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B29" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E29" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B30" s="2" t="b">
         <v>0</v>
@@ -3844,32 +3859,32 @@
         <v>0</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B31" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B32" s="2" t="b">
         <v>0</v>
@@ -3878,32 +3893,32 @@
         <v>0</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B33" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E33" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B34" s="2" t="b">
         <v>0</v>
@@ -3912,32 +3927,32 @@
         <v>0</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B35" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B36" s="2" t="b">
         <v>0</v>
@@ -3946,32 +3961,32 @@
         <v>0</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B37" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E37" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B38" s="2" t="b">
         <v>0</v>
@@ -3980,15 +3995,15 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B39" s="2" t="b">
         <v>0</v>
@@ -3997,49 +4012,49 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B40" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E40" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B41" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B42" s="2" t="b">
         <v>0</v>
@@ -4048,49 +4063,49 @@
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B43" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E43" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B44" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B45" s="2" t="b">
         <v>0</v>
@@ -4099,15 +4114,15 @@
         <v>0</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B46" s="2" t="b">
         <v>0</v>
@@ -4116,15 +4131,15 @@
         <v>0</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B47" s="2" t="b">
         <v>0</v>
@@ -4133,15 +4148,15 @@
         <v>0</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B48" s="2" t="b">
         <v>0</v>
@@ -4150,32 +4165,32 @@
         <v>0</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B49" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E49" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B50" s="2" t="b">
         <v>0</v>
@@ -4184,32 +4199,32 @@
         <v>0</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B51" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E51" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>86</v>
+        <v>146</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B52" s="2" t="b">
         <v>0</v>
@@ -4218,15 +4233,15 @@
         <v>0</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B53" s="2" t="b">
         <v>0</v>
@@ -4235,15 +4250,15 @@
         <v>0</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B54" s="2" t="b">
         <v>0</v>
@@ -4252,15 +4267,15 @@
         <v>0</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B55" s="2" t="b">
         <v>0</v>
@@ -4269,15 +4284,15 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B56" s="2" t="b">
         <v>0</v>
@@ -4286,32 +4301,32 @@
         <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B57" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E57" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B58" s="2" t="b">
         <v>0</v>
@@ -4320,83 +4335,83 @@
         <v>0</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B59" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E59" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>170</v>
+        <v>93</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B60" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E60" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B61" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E61" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B62" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E62" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B63" s="2" t="b">
         <v>0</v>
@@ -4405,15 +4420,15 @@
         <v>1</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B64" s="2" t="b">
         <v>0</v>
@@ -4422,106 +4437,140 @@
         <v>0</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B65" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E65" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B66" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E66" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B67" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E67" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>314</v>
+        <v>191</v>
       </c>
       <c r="B68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D68" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="F68" s="2" t="s">
-        <v>315</v>
+        <v>192</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>316</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B69" s="2" t="b">
+      <c r="B71" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D69" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" s="2" t="s">
+      <c r="C71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>316</v>
       </c>
     </row>

</xml_diff>

<commit_message>
numerous bug fixes, some related to #6
</commit_message>
<xml_diff>
--- a/formative-elements/formative-elements.xlsx
+++ b/formative-elements/formative-elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\working_copies\SoilTaxonomy\formative-elements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C1A4ED-8493-46BF-97C3-E8EB6BB6C52D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C350BE-FE36-4D8D-9609-542D178ACCCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9780" activeTab="3" xr2:uid="{728FE064-2144-4183-8F3E-A5F6ED41A2A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9780" activeTab="1" xr2:uid="{728FE064-2144-4183-8F3E-A5F6ED41A2A3}"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="455">
   <si>
     <t>element</t>
   </si>
@@ -1395,6 +1395,9 @@
   </si>
   <si>
     <t>more aridic than typic subgroup</t>
+  </si>
+  <si>
+    <t>ist</t>
   </si>
 </sst>
 </file>
@@ -1980,10 +1983,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2406C0-4B40-475B-B0B2-D2A68ED4FB2E}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2191,155 +2194,166 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>282</v>
+        <v>454</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>93</v>
+        <v>226</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>285</v>
+        <v>93</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>34</v>
+        <v>288</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>293</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>86</v>
+        <v>293</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>152</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>154</v>
+        <v>86</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>298</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>300</v>
+        <v>154</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>439</v>
+        <v>298</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>174</v>
+        <v>300</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>302</v>
+        <v>439</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>31</v>
+        <v>189</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3325,7 +3339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D2594B-1AEA-4072-B7F9-758DAECAB91F}">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
found all missing subgroup formative elements, plent yet todo
</commit_message>
<xml_diff>
--- a/formative-elements/formative-elements.xlsx
+++ b/formative-elements/formative-elements.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\working_copies\SoilTaxonomy\formative-elements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C350BE-FE36-4D8D-9609-542D178ACCCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB42BB36-3A73-4F27-A3E9-5EB5EBB7A91C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9780" activeTab="1" xr2:uid="{728FE064-2144-4183-8F3E-A5F6ED41A2A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9780" activeTab="4" xr2:uid="{728FE064-2144-4183-8F3E-A5F6ED41A2A3}"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="2" r:id="rId1"/>
     <sheet name="suborder" sheetId="3" r:id="rId2"/>
     <sheet name="greatgroup" sheetId="4" r:id="rId3"/>
     <sheet name="subgroup" sheetId="1" r:id="rId4"/>
+    <sheet name="subgroup-pending" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="552">
   <si>
     <t>element</t>
   </si>
@@ -116,9 +117,6 @@
     <t>human controlled flooding as in paddy rice culture</t>
   </si>
   <si>
-    <t>antropic</t>
-  </si>
-  <si>
     <t>human</t>
   </si>
   <si>
@@ -461,9 +459,6 @@
     <t>presence of a placic horizon</t>
   </si>
   <si>
-    <t>plinthitic</t>
-  </si>
-  <si>
     <t>brick</t>
   </si>
   <si>
@@ -1398,6 +1393,303 @@
   </si>
   <si>
     <t>ist</t>
+  </si>
+  <si>
+    <t>entic</t>
+  </si>
+  <si>
+    <t>minimal surface/subsurface development</t>
+  </si>
+  <si>
+    <t>alfic</t>
+  </si>
+  <si>
+    <t>presence of an argillic or kandic horizon</t>
+  </si>
+  <si>
+    <t>anthropic</t>
+  </si>
+  <si>
+    <t>plinthic</t>
+  </si>
+  <si>
+    <t>acraquoxic</t>
+  </si>
+  <si>
+    <t>acrudoxic</t>
+  </si>
+  <si>
+    <t>acrustoxic</t>
+  </si>
+  <si>
+    <t>albaquultic</t>
+  </si>
+  <si>
+    <t>andic</t>
+  </si>
+  <si>
+    <t>anhydritic</t>
+  </si>
+  <si>
+    <t>anthraltic</t>
+  </si>
+  <si>
+    <t>anthrodensic</t>
+  </si>
+  <si>
+    <t>anthroportic</t>
+  </si>
+  <si>
+    <t>aqualfic</t>
+  </si>
+  <si>
+    <t>aquandic</t>
+  </si>
+  <si>
+    <t>aquentic</t>
+  </si>
+  <si>
+    <t>aqueptic</t>
+  </si>
+  <si>
+    <t>aquertic</t>
+  </si>
+  <si>
+    <t>aquicambidic</t>
+  </si>
+  <si>
+    <t>aquodic</t>
+  </si>
+  <si>
+    <t>aquollic</t>
+  </si>
+  <si>
+    <t>aquultic</t>
+  </si>
+  <si>
+    <t>argiaquic</t>
+  </si>
+  <si>
+    <t>argidic</t>
+  </si>
+  <si>
+    <t>argiduridic</t>
+  </si>
+  <si>
+    <t>calciargidic</t>
+  </si>
+  <si>
+    <t>calcidic</t>
+  </si>
+  <si>
+    <t>cambidic</t>
+  </si>
+  <si>
+    <t>duridic</t>
+  </si>
+  <si>
+    <t>fluventic</t>
+  </si>
+  <si>
+    <t>folistic</t>
+  </si>
+  <si>
+    <t>grossic</t>
+  </si>
+  <si>
+    <t>haplargidic</t>
+  </si>
+  <si>
+    <t>haplocalcidic</t>
+  </si>
+  <si>
+    <t>haploduridic</t>
+  </si>
+  <si>
+    <t>haploplaggic</t>
+  </si>
+  <si>
+    <t>haploxeralfic</t>
+  </si>
+  <si>
+    <t>haploxerandic</t>
+  </si>
+  <si>
+    <t>haploxerollic</t>
+  </si>
+  <si>
+    <t>haplustandic</t>
+  </si>
+  <si>
+    <t>histic</t>
+  </si>
+  <si>
+    <t>humaqueptic</t>
+  </si>
+  <si>
+    <t>hydraquentic</t>
+  </si>
+  <si>
+    <t>inceptic</t>
+  </si>
+  <si>
+    <t>kandiudalfic</t>
+  </si>
+  <si>
+    <t>kandiustalfic</t>
+  </si>
+  <si>
+    <t>kanhaplic</t>
+  </si>
+  <si>
+    <t>lithic-ruptic-entic</t>
+  </si>
+  <si>
+    <t>mollic</t>
+  </si>
+  <si>
+    <t>natrargidic</t>
+  </si>
+  <si>
+    <t>natrixeralfic</t>
+  </si>
+  <si>
+    <t>oxic</t>
+  </si>
+  <si>
+    <t>paleargidic</t>
+  </si>
+  <si>
+    <t>palexerollic</t>
+  </si>
+  <si>
+    <t>petrocalcidic</t>
+  </si>
+  <si>
+    <t>plinthaquic</t>
+  </si>
+  <si>
+    <t>psammentic</t>
+  </si>
+  <si>
+    <t>rendollic</t>
+  </si>
+  <si>
+    <t>ruptic-alfic</t>
+  </si>
+  <si>
+    <t>ruptic-entic</t>
+  </si>
+  <si>
+    <t>ruptic-histic</t>
+  </si>
+  <si>
+    <t>ruptic-inceptic</t>
+  </si>
+  <si>
+    <t>ruptic-lithic</t>
+  </si>
+  <si>
+    <t>ruptic-ultic</t>
+  </si>
+  <si>
+    <t>salidic</t>
+  </si>
+  <si>
+    <t>spodic</t>
+  </si>
+  <si>
+    <t>sulfaqueptic</t>
+  </si>
+  <si>
+    <t>sulfuric</t>
+  </si>
+  <si>
+    <t>thapto-histic</t>
+  </si>
+  <si>
+    <t>torrertic</t>
+  </si>
+  <si>
+    <t>torrifluventic</t>
+  </si>
+  <si>
+    <t>torriorthentic</t>
+  </si>
+  <si>
+    <t>torripsammentic</t>
+  </si>
+  <si>
+    <t>torroxic</t>
+  </si>
+  <si>
+    <t>udandic</t>
+  </si>
+  <si>
+    <t>udertic</t>
+  </si>
+  <si>
+    <t>udifluventic</t>
+  </si>
+  <si>
+    <t>udollic</t>
+  </si>
+  <si>
+    <t>udorthentic</t>
+  </si>
+  <si>
+    <t>udoxic</t>
+  </si>
+  <si>
+    <t>ultic</t>
+  </si>
+  <si>
+    <t>ustalfic</t>
+  </si>
+  <si>
+    <t>ustandic</t>
+  </si>
+  <si>
+    <t>ustertic</t>
+  </si>
+  <si>
+    <t>ustifluventic</t>
+  </si>
+  <si>
+    <t>ustivitrandic</t>
+  </si>
+  <si>
+    <t>ustollic</t>
+  </si>
+  <si>
+    <t>ustoxic</t>
+  </si>
+  <si>
+    <t>vertic</t>
+  </si>
+  <si>
+    <t>vitrandic</t>
+  </si>
+  <si>
+    <t>vitritorrandic</t>
+  </si>
+  <si>
+    <t>vitrixerandic</t>
+  </si>
+  <si>
+    <t>xeralfic</t>
+  </si>
+  <si>
+    <t>xereptic</t>
+  </si>
+  <si>
+    <t>xerertic</t>
+  </si>
+  <si>
+    <t>xerofluventic</t>
+  </si>
+  <si>
+    <t>xerollic</t>
   </si>
 </sst>
 </file>
@@ -1775,7 +2067,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1790,7 +2082,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1805,175 +2097,175 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -1985,7 +2277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2406C0-4B40-475B-B0B2-D2A68ED4FB2E}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2013,348 +2305,348 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2366,7 +2658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4648FD0D-CFBB-44A9-AB17-265531B6E9AE}">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2392,942 +2684,942 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>350</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>367</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>392</v>
-      </c>
       <c r="C47" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>399</v>
-      </c>
       <c r="C50" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>398</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>412</v>
-      </c>
       <c r="C57" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>422</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>437</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -3337,10 +3629,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D2594B-1AEA-4072-B7F9-758DAECAB91F}">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3362,16 +3654,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -3383,7 +3675,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3465,7 +3757,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>18</v>
@@ -3473,24 +3765,24 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>455</v>
       </c>
       <c r="B7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>197</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>20</v>
+        <v>456</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>0</v>
@@ -3499,15 +3791,15 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2" t="b">
         <v>0</v>
@@ -3516,15 +3808,15 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="b">
         <v>0</v>
@@ -3533,32 +3825,32 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>457</v>
       </c>
       <c r="B11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="b">
         <v>0</v>
@@ -3567,15 +3859,15 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2" t="b">
         <v>0</v>
@@ -3584,15 +3876,15 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>452</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2" t="b">
         <v>0</v>
@@ -3601,49 +3893,49 @@
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>300</v>
+        <v>36</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>453</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>450</v>
       </c>
       <c r="B15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>40</v>
+        <v>298</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>41</v>
+        <v>451</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B17" s="2" t="b">
         <v>0</v>
@@ -3652,32 +3944,32 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" s="2" t="b">
         <v>0</v>
@@ -3686,32 +3978,32 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="b">
         <v>0</v>
@@ -3720,32 +4012,32 @@
         <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>453</v>
       </c>
       <c r="B22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>63</v>
+        <v>200</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>91</v>
+        <v>454</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>449</v>
+        <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
         <v>0</v>
@@ -3754,15 +4046,15 @@
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>450</v>
+        <v>56</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>451</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B24" s="2" t="b">
         <v>0</v>
@@ -3771,32 +4063,32 @@
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>67</v>
+        <v>447</v>
       </c>
       <c r="B25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E25" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>68</v>
+        <v>448</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>69</v>
+        <v>449</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="b">
         <v>0</v>
@@ -3805,15 +4097,15 @@
         <v>0</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B27" s="2" t="b">
         <v>0</v>
@@ -3822,15 +4114,15 @@
         <v>0</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B28" s="2" t="b">
         <v>0</v>
@@ -3839,32 +4131,32 @@
         <v>0</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B29" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E29" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B30" s="2" t="b">
         <v>0</v>
@@ -3873,32 +4165,32 @@
         <v>0</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B31" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B32" s="2" t="b">
         <v>0</v>
@@ -3907,32 +4199,32 @@
         <v>0</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B33" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E33" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B34" s="2" t="b">
         <v>0</v>
@@ -3941,32 +4233,32 @@
         <v>0</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B36" s="2" t="b">
         <v>0</v>
@@ -3975,32 +4267,32 @@
         <v>0</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B37" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E37" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B38" s="2" t="b">
         <v>0</v>
@@ -4009,32 +4301,32 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B39" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B40" s="2" t="b">
         <v>0</v>
@@ -4043,15 +4335,15 @@
         <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B41" s="2" t="b">
         <v>0</v>
@@ -4060,49 +4352,49 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B42" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B43" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E43" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B44" s="2" t="b">
         <v>0</v>
@@ -4111,49 +4403,49 @@
         <v>1</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B45" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B46" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B47" s="2" t="b">
         <v>0</v>
@@ -4162,15 +4454,15 @@
         <v>0</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B48" s="2" t="b">
         <v>0</v>
@@ -4179,15 +4471,15 @@
         <v>0</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B49" s="2" t="b">
         <v>0</v>
@@ -4196,15 +4488,15 @@
         <v>0</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B50" s="2" t="b">
         <v>0</v>
@@ -4213,32 +4505,32 @@
         <v>0</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B51" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E51" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>148</v>
+        <v>458</v>
       </c>
       <c r="B52" s="2" t="b">
         <v>0</v>
@@ -4247,32 +4539,32 @@
         <v>0</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B53" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E53" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B54" s="2" t="b">
         <v>0</v>
@@ -4281,15 +4573,15 @@
         <v>0</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B55" s="2" t="b">
         <v>0</v>
@@ -4298,15 +4590,15 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B56" s="2" t="b">
         <v>0</v>
@@ -4315,15 +4607,15 @@
         <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B57" s="2" t="b">
         <v>0</v>
@@ -4332,15 +4624,15 @@
         <v>0</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B58" s="2" t="b">
         <v>0</v>
@@ -4349,32 +4641,32 @@
         <v>0</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B59" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E59" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B60" s="2" t="b">
         <v>0</v>
@@ -4383,83 +4675,83 @@
         <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B61" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E61" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>170</v>
+        <v>92</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B62" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E62" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B63" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E63" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B64" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E64" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B65" s="2" t="b">
         <v>0</v>
@@ -4468,15 +4760,15 @@
         <v>1</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B66" s="2" t="b">
         <v>0</v>
@@ -4485,111 +4777,665 @@
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B67" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E67" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B68" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E68" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B69" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E69" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>314</v>
+        <v>189</v>
       </c>
       <c r="B70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D70" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="F70" s="2" t="s">
-        <v>315</v>
+        <v>190</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>316</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>317</v>
+        <v>192</v>
       </c>
       <c r="B71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D71" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="F71" s="2" t="s">
-        <v>318</v>
+        <v>193</v>
       </c>
       <c r="G71" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B72" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>316</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35D6C17-BEAA-4913-B02D-3E7B5BD5E340}">
+  <dimension ref="A1:I94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="9.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="15.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="49" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.28515625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>